<commit_message>
Filter specimens missing coordinates and add expr() call around ggplot object.
</commit_message>
<xml_diff>
--- a/data/map-labels.xlsx
+++ b/data/map-labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonratcliff/Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BC2CD5-D160-1243-ADCE-73D66DEA7A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E8F86A-69BC-F648-B0F4-1040428101AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19380" yWindow="2080" windowWidth="13780" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19820" yWindow="460" windowWidth="13780" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,11 +288,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,10 +635,10 @@
   <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -671,10 +672,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C4">
-        <v>-0.3</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -693,10 +694,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-0.4</v>
+        <v>-0.25</v>
       </c>
       <c r="C6">
-        <v>-0.2</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -704,10 +705,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.2</v>
+        <v>-0.15</v>
       </c>
       <c r="C7">
-        <v>-0.25</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -715,36 +716,54 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C8">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>0.3</v>
+      </c>
+      <c r="C9">
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>0.3</v>
+      </c>
+      <c r="C10">
+        <v>-0.2</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="C12">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -763,10 +782,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="C14">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -785,10 +804,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>-0.3</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -796,10 +815,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="C17">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -810,25 +829,37 @@
         <v>0.25</v>
       </c>
       <c r="C18">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="C21">
         <v>-0.2</v>
@@ -838,26 +869,44 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
+      <c r="B22">
+        <v>0.4</v>
+      </c>
+      <c r="C22">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+      <c r="C23">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="C24">
+        <v>-0.2</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-0.25</v>
+        <v>-0.2</v>
       </c>
       <c r="C25">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -865,7 +914,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="C26">
         <v>-0.27500000000000002</v>
@@ -875,11 +924,23 @@
       <c r="A27" t="s">
         <v>26</v>
       </c>
+      <c r="B27">
+        <v>0.45</v>
+      </c>
+      <c r="C27">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
+      <c r="B28">
+        <v>0.45</v>
+      </c>
+      <c r="C28">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -897,7 +958,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>0.3</v>
@@ -919,10 +980,10 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>-0.35</v>
+        <v>-0.45</v>
       </c>
       <c r="C32">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -930,26 +991,32 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>-0.27500000000000002</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
+      <c r="B34">
+        <v>0.5</v>
+      </c>
+      <c r="C34">
+        <v>-0.15</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="C35">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -957,26 +1024,32 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-0.4</v>
+        <v>-0.3</v>
       </c>
       <c r="C36">
-        <v>-0.2</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
+      <c r="B37">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="C37">
+        <v>-0.15</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="C38">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -984,26 +1057,32 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C39">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
+      <c r="B40">
+        <v>-0.65</v>
+      </c>
+      <c r="C40">
+        <v>-0.05</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.4</v>
+        <v>-0.3</v>
       </c>
       <c r="C41">
-        <v>-0.2</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1011,7 +1090,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C42">
         <v>-0.2</v>
@@ -1022,10 +1101,10 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.1</v>
+        <v>-0.15</v>
       </c>
       <c r="C43">
-        <v>0.25</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1033,10 +1112,10 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>-0.25</v>
+        <v>-0.6</v>
       </c>
       <c r="C44">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1044,31 +1123,43 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>-0.45</v>
       </c>
       <c r="C45">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
+      <c r="B46">
+        <v>0.5</v>
+      </c>
+      <c r="C46">
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
+      <c r="B47">
+        <v>0.35</v>
+      </c>
+      <c r="C47">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48">
-        <v>0.35</v>
+      <c r="B48" s="2">
+        <v>-0.35</v>
       </c>
       <c r="C48">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1079,7 +1170,7 @@
         <v>0.25</v>
       </c>
       <c r="C49">
-        <v>-0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -1097,18 +1188,30 @@
       <c r="A51" t="s">
         <v>50</v>
       </c>
+      <c r="B51">
+        <v>-0.5</v>
+      </c>
+      <c r="C51">
+        <v>-0.1</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
+      <c r="B52">
+        <v>-0.5</v>
+      </c>
+      <c r="C52">
+        <v>-0.2</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53">
-        <v>-0.25</v>
+        <v>-0.3</v>
       </c>
       <c r="C53">
         <v>0.25</v>
@@ -1124,7 +1227,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>-0.3</v>
+        <v>-0.25</v>
       </c>
       <c r="C55">
         <v>-0.2</v>
@@ -1135,7 +1238,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C56">
         <v>0.05</v>
@@ -1171,7 +1274,7 @@
         <v>-0.25</v>
       </c>
       <c r="C59">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1179,28 +1282,40 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>-0.45</v>
+        <v>-0.5</v>
       </c>
       <c r="C60">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
+      <c r="B62">
+        <v>-0.5</v>
+      </c>
+      <c r="C62">
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-0.25</v>
+        <v>0.05</v>
       </c>
       <c r="C63">
         <v>-0.25</v>
@@ -1211,10 +1326,10 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>0.5</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="C64">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1225,13 +1340,19 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>-0.2</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>-0.4</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -1259,11 +1380,23 @@
       <c r="A69" t="s">
         <v>67</v>
       </c>
+      <c r="B69">
+        <v>0.35</v>
+      </c>
+      <c r="C69">
+        <v>-0.2</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
+      <c r="B70">
+        <v>0.3</v>
+      </c>
+      <c r="C70">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -1290,6 +1423,12 @@
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
+      </c>
+      <c r="B73">
+        <v>-0.2</v>
+      </c>
+      <c r="C73">
+        <v>-0.25</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update label positions and plot size.
</commit_message>
<xml_diff>
--- a/data/map-labels.xlsx
+++ b/data/map-labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonratcliff/Thesis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E8F86A-69BC-F648-B0F4-1040428101AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF99B268-709C-F641-BF4D-BF998748BA4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19820" yWindow="460" windowWidth="13780" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -635,10 +635,10 @@
   <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1049,7 +1049,7 @@
         <v>-0.25</v>
       </c>
       <c r="C38">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1071,7 +1071,7 @@
         <v>-0.65</v>
       </c>
       <c r="C40">
-        <v>-0.05</v>
+        <v>-0.15</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1079,7 +1079,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.3</v>
+        <v>-0.4</v>
       </c>
       <c r="C41">
         <v>-0.25</v>
@@ -1159,7 +1159,7 @@
         <v>-0.35</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -1381,7 +1381,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="C69">
         <v>-0.2</v>

</xml_diff>